<commit_message>
updating documentation and cleaning up
</commit_message>
<xml_diff>
--- a/Planning/Gantt.xlsx
+++ b/Planning/Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin\Documents\CNU\spring2021\capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin\Documents\CNU\capstone\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC885E1F-7D17-4F4A-98D7-3D65500F376F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5F677B-7F7B-4259-B971-DFA8E133D827}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1860" windowWidth="17280" windowHeight="8652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -621,6 +621,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -628,12 +634,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1377,8 +1377,8 @@
   </sheetPr>
   <dimension ref="B1:AJ33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1455,22 +1455,22 @@
       <c r="AJ2" s="22"/>
     </row>
     <row r="3" spans="2:36" s="11" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="37" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1497,12 +1497,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1555,10 +1555,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="7">
         <v>0</v>
@@ -1585,10 +1585,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
@@ -1618,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="7">
         <v>0</v>
@@ -1645,10 +1645,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
@@ -1675,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -1735,10 +1735,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" s="7">
         <v>0</v>
@@ -1765,10 +1765,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="7">
         <v>0</v>
@@ -1885,10 +1885,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="7">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -2035,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>

</xml_diff>